<commit_message>
alte Übersetzungen entfernt und kleinere Anpassungen
</commit_message>
<xml_diff>
--- a/output/ValueSet-t-cabs-valueset-Beatmungsmodus.xlsx
+++ b/output/ValueSet-t-cabs-valueset-Beatmungsmodus.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-19T11:55:29+01:00</t>
+    <t>2025-11-20T17:13:04+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>MDC_VENT_MODE_ISO_HIFLOW_3NIV</t>
+  </si>
+  <si>
+    <t>475155</t>
+  </si>
+  <si>
+    <t>MDC_VENT_MODE_ISO_CSV_vtPS_6ACAP_012_015</t>
+  </si>
+  <si>
+    <t>475144</t>
+  </si>
+  <si>
+    <t>MDC_VENT_MODE_ISO_SIMV_PC_8PS_6ACAP</t>
   </si>
   <si>
     <t/>
@@ -430,7 +442,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -533,15 +545,31 @@
         <v>48</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>